<commit_message>
Further development chapter tidy data.
</commit_message>
<xml_diff>
--- a/practicefiles/Tidy003.xlsx
+++ b/practicefiles/Tidy003.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\office\LearnExcel-source\practicefiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1118B7FF-B305-4A52-90D2-F24891BE9EF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C517B3F-EFE2-46C1-869A-C23E35801698}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E924E56E-C614-4139-B318-8A69E85F72ED}"/>
   </bookViews>
@@ -50,13 +50,13 @@
     <t>English</t>
   </si>
   <si>
-    <t>Maths</t>
-  </si>
-  <si>
     <t>Year</t>
   </si>
   <si>
     <t>Test</t>
+  </si>
+  <si>
+    <t>Math</t>
   </si>
 </sst>
 </file>
@@ -411,7 +411,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -426,10 +426,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -446,7 +446,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C2">
         <v>2017</v>
@@ -466,7 +466,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C3">
         <v>2018</v>
@@ -526,7 +526,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C6">
         <v>2017</v>
@@ -546,7 +546,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C7">
         <v>2018</v>
@@ -606,7 +606,7 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C10">
         <v>2017</v>
@@ -626,7 +626,7 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C11">
         <v>2018</v>

</xml_diff>